<commit_message>
Excel signup sheet added
</commit_message>
<xml_diff>
--- a/Onlylearning/Onlylearning/Input/SkillParticulars.xlsx
+++ b/Onlylearning/Onlylearning/Input/SkillParticulars.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/35cd48efcf2af70f/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="11_F25DC773A252ABDACC1048EBF95F52EA5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6F5E993-5E64-4EEE-B200-6414C18DEF15}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="11_F25DC773A252ABDACC1048EBF95F52EA5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{738106F7-947F-4AD5-985E-1CD4CFC8E8EA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7400" yWindow="1070" windowWidth="11020" windowHeight="8820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SkillsProfile" sheetId="1" r:id="rId1"/>
+    <sheet name="Signup" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Title</t>
   </si>
@@ -114,13 +115,40 @@
   </si>
   <si>
     <t>To speak good English you need to think in English</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>testingroro1@gmail.com</t>
+  </si>
+  <si>
+    <t>hello123</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lastname </t>
+  </si>
+  <si>
+    <t>Munni</t>
+  </si>
+  <si>
+    <t>Roro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +161,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,10 +188,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -168,8 +205,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,8 +493,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -535,10 +577,10 @@
         <v>12</v>
       </c>
       <c r="H2" s="4">
-        <v>44895</v>
+        <v>44909</v>
       </c>
       <c r="I2" s="3">
-        <v>44895</v>
+        <v>44909</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -546,8 +588,8 @@
       <c r="K2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L2">
-        <v>30</v>
+      <c r="L2" s="6">
+        <v>3</v>
       </c>
       <c r="M2" t="s">
         <v>20</v>
@@ -568,4 +610,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC76822-F99C-4F22-A0A2-85AC2909A150}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2E6966D5-EDA6-4126-9949-1299ECAC4E87}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>